<commit_message>
MFY auto commit at 30/05/2022 10:19:54
</commit_message>
<xml_diff>
--- a/Marks.xlsx
+++ b/Marks.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DarkJoker\Desktop\Semeste_6_FALL-2021_\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{061F7731-4AE7-41C7-BAEF-1EDE753E8C93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C2EBC40-53FD-41AE-B2F6-B7B3903B9F1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GPA" sheetId="7" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="23">
   <si>
     <t>Project</t>
   </si>
@@ -172,7 +172,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -191,6 +191,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -664,7 +667,7 @@
   <dimension ref="B4:J16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12:J12"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.2"/>
@@ -677,12 +680,12 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="G4" s="8" t="s">
+      <c r="G4" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
     </row>
     <row r="5" spans="2:10" ht="31.5" x14ac:dyDescent="0.2">
       <c r="C5" s="2" t="s">
@@ -800,10 +803,14 @@
       </c>
       <c r="E11" s="1">
         <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="F11" s="2">
-        <v>14</v>
+        <v>17</v>
+      </c>
+      <c r="F11" s="8">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="G11" s="1">
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.2">
@@ -818,14 +825,14 @@
       </c>
       <c r="E12" s="1">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F12" s="2">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G12" s="1">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.2">
@@ -843,7 +850,7 @@
       <c r="D14" s="2"/>
       <c r="E14" s="3">
         <f>ROUND(SUM(E7:E12),2)</f>
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F14" s="3" t="str">
         <f>IF(E14&gt;86,"A",IF(E14&gt;82,"A-",IF(E14&gt;78,"B+",IF(E14&gt;74,"B",IF(E14&gt;70,"B-",IF(E14&gt;66,"C+",IF(E14&gt;62,"C",IF(E14&gt;58,"C-","F"))))))))</f>
@@ -865,10 +872,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="B5:M15"/>
+  <dimension ref="B5:N15"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -876,7 +883,7 @@
     <col min="1" max="256" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:13" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:14" ht="31.5" x14ac:dyDescent="0.2">
       <c r="B5" s="1"/>
       <c r="C5" s="2" t="s">
         <v>6</v>
@@ -902,8 +909,20 @@
       <c r="J5" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="2:13" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="K5" s="8">
+        <v>5</v>
+      </c>
+      <c r="L5" s="8">
+        <v>6</v>
+      </c>
+      <c r="M5" s="8">
+        <v>7</v>
+      </c>
+      <c r="N5" s="8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -913,7 +932,7 @@
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
     </row>
-    <row r="7" spans="2:13" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:14" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="1"/>
@@ -924,7 +943,7 @@
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
     </row>
-    <row r="8" spans="2:13" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:14" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
         <v>1</v>
       </c>
@@ -932,39 +951,31 @@
         <v>15</v>
       </c>
       <c r="D8" s="1">
-        <v>70</v>
+        <v>45</v>
       </c>
       <c r="E8" s="1">
         <f>ROUND((F8/D8)*C8,2)</f>
-        <v>9.43</v>
+        <v>13.67</v>
       </c>
       <c r="F8" s="2">
         <f>SUM(G8:M8)</f>
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G8" s="1">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="H8" s="1">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="I8" s="1">
-        <v>7</v>
-      </c>
-      <c r="J8" s="1">
-        <v>7</v>
-      </c>
-      <c r="K8" s="1">
-        <v>6</v>
-      </c>
-      <c r="L8" s="1">
-        <v>5</v>
-      </c>
-      <c r="M8" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="2:13" ht="15.75" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+    </row>
+    <row r="9" spans="2:14" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B9" s="2" t="s">
         <v>2</v>
       </c>
@@ -972,38 +983,41 @@
         <v>15</v>
       </c>
       <c r="D9" s="1">
-        <v>50</v>
+        <v>250</v>
       </c>
       <c r="E9" s="1">
         <f t="shared" ref="E9:E11" si="0">(F9/D9)*C9</f>
-        <v>15</v>
+        <v>13.68</v>
       </c>
       <c r="F9" s="2">
         <f t="shared" ref="F9:F11" si="1">SUM(G9:M9)</f>
+        <v>228</v>
+      </c>
+      <c r="G9" s="1">
+        <v>29</v>
+      </c>
+      <c r="H9" s="1">
+        <v>29</v>
+      </c>
+      <c r="I9" s="1">
+        <v>27</v>
+      </c>
+      <c r="J9" s="1">
+        <v>25</v>
+      </c>
+      <c r="K9" s="1">
         <v>50</v>
       </c>
-      <c r="G9" s="1">
-        <v>10</v>
-      </c>
-      <c r="H9" s="1">
-        <v>10</v>
-      </c>
-      <c r="I9" s="1">
-        <v>10</v>
-      </c>
-      <c r="J9" s="1">
-        <v>10</v>
-      </c>
-      <c r="K9" s="1">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="2:13" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="L9" s="1">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B10" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C10" s="2">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="D10" s="1">
         <v>60</v>
@@ -1021,7 +1035,7 @@
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
     </row>
-    <row r="11" spans="2:13" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:14" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
         <v>4</v>
       </c>
@@ -1046,7 +1060,7 @@
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
     </row>
-    <row r="12" spans="2:13" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:14" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="1"/>
@@ -1057,7 +1071,7 @@
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
     </row>
-    <row r="13" spans="2:13" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:14" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -1068,18 +1082,18 @@
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
     </row>
-    <row r="14" spans="2:13" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:14" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B14" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C14" s="2">
         <f>SUM(C7:C12)</f>
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2">
         <f>ROUND(SUM(E7:E12),2)</f>
-        <v>42.93</v>
+        <v>45.85</v>
       </c>
       <c r="F14" s="1" t="str">
         <f>IF(E14&gt;86,"A",IF(E14&gt;82,"A-",IF(E14&gt;78,"B+",IF(E14&gt;74,"B",IF(E14&gt;70,"B-",IF(E14&gt;66,"C+",IF(E14&gt;62,"C",IF(E14&gt;58,"C-","F"))))))))</f>
@@ -1090,7 +1104,7 @@
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
     </row>
-    <row r="15" spans="2:13" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:14" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -1110,7 +1124,7 @@
   <dimension ref="B5:J15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:G7"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1284,14 +1298,14 @@
       </c>
       <c r="E12" s="1">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F12" s="2">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G12" s="1">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
@@ -1319,7 +1333,7 @@
       <c r="D14" s="2"/>
       <c r="E14" s="2">
         <f>ROUND(SUM(E7:E12),2)</f>
-        <v>23.8</v>
+        <v>18.8</v>
       </c>
       <c r="F14" s="1" t="str">
         <f>IF(E14&gt;86,"A",IF(E14&gt;82,"A-",IF(E14&gt;78,"B+",IF(E14&gt;74,"B",IF(E14&gt;70,"B-",IF(E14&gt;66,"C+",IF(E14&gt;62,"C",IF(E14&gt;58,"C-","F"))))))))</f>
@@ -1349,8 +1363,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B5:J60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:H6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1443,14 +1457,14 @@
       </c>
       <c r="E8" s="1">
         <f t="shared" ref="E8:E10" si="0">(F8/D8)*C8</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F8" s="2">
         <f t="shared" ref="F8:F10" si="1">SUM(G8:M8)</f>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="G8" s="1">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
@@ -1526,7 +1540,7 @@
       <c r="D12" s="2"/>
       <c r="E12" s="2">
         <f>ROUND(SUM(E7:E10),2)</f>
-        <v>22.5</v>
+        <v>17.5</v>
       </c>
       <c r="F12" s="1" t="str">
         <f>IF(E12&gt;86,"A",IF(E12&gt;82,"A-",IF(E12&gt;78,"B+",IF(E12&gt;74,"B",IF(E12&gt;70,"B-",IF(E12&gt;66,"C+",IF(E12&gt;62,"C",IF(E12&gt;58,"C-","F"))))))))</f>
@@ -1562,7 +1576,7 @@
   <dimension ref="B5:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B11" sqref="B11:G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1602,7 +1616,7 @@
         <v>0</v>
       </c>
       <c r="C6" s="7">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D6" s="1">
         <v>15</v>
@@ -1625,18 +1639,18 @@
         <v>1</v>
       </c>
       <c r="C7" s="2">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D7" s="1">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="E7" s="1">
         <f>ROUND((F7/D7)*C7,2)</f>
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F7" s="2">
         <f>SUM(G7:M7)</f>
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="G7" s="1">
         <v>16</v>
@@ -1644,7 +1658,9 @@
       <c r="H7" s="1">
         <v>12</v>
       </c>
-      <c r="I7" s="1"/>
+      <c r="I7" s="1">
+        <v>12</v>
+      </c>
       <c r="J7" s="1"/>
     </row>
     <row r="8" spans="2:10" ht="15.75" x14ac:dyDescent="0.2">
@@ -1652,20 +1668,22 @@
         <v>2</v>
       </c>
       <c r="C8" s="2">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D8" s="1">
         <v>20</v>
       </c>
       <c r="E8" s="1">
         <f t="shared" ref="E8:E11" si="0">(F8/D8)*C8</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="F8" s="2">
         <f t="shared" ref="F8:F11" si="1">SUM(G8:M8)</f>
-        <v>0</v>
-      </c>
-      <c r="G8" s="1"/>
+        <v>20</v>
+      </c>
+      <c r="G8" s="1">
+        <v>20</v>
+      </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
@@ -1719,26 +1737,12 @@
       <c r="J10" s="1"/>
     </row>
     <row r="11" spans="2:10" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="B11" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" s="7">
-        <v>5</v>
-      </c>
-      <c r="D11" s="1">
-        <v>5</v>
-      </c>
-      <c r="E11" s="1">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="F11" s="7">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="G11" s="1">
-        <v>5</v>
-      </c>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
@@ -1758,7 +1762,7 @@
       <c r="D13" s="2"/>
       <c r="E13" s="2">
         <f>ROUND(SUM(E6:E11),2)</f>
-        <v>29.5</v>
+        <v>42.5</v>
       </c>
       <c r="F13" s="1" t="str">
         <f>IF(E13&gt;86,"A",IF(E13&gt;82,"A-",IF(E13&gt;78,"B+",IF(E13&gt;74,"B",IF(E13&gt;70,"B-",IF(E13&gt;66,"C+",IF(E13&gt;62,"C",IF(E13&gt;58,"C-","F"))))))))</f>
@@ -1778,8 +1782,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAAB841F-FB29-4B50-A6D0-F2C50CE00124}">
   <dimension ref="B5:J13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6:G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1815,26 +1819,11 @@
       </c>
     </row>
     <row r="6" spans="2:10" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="B6" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C6" s="7">
-        <v>15</v>
-      </c>
-      <c r="D6" s="1">
-        <v>10</v>
-      </c>
-      <c r="E6" s="1">
-        <f>(F6/D6)*C6</f>
-        <v>15</v>
-      </c>
-      <c r="F6" s="7">
-        <f>SUM(G6:M6)</f>
-        <v>10</v>
-      </c>
-      <c r="G6" s="1">
-        <v>10</v>
-      </c>
+      <c r="C6" s="7"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
@@ -1844,18 +1833,18 @@
         <v>1</v>
       </c>
       <c r="C7" s="7">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D7" s="1">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="E7" s="1">
         <f>ROUND((F7/D7)*C7,2)</f>
-        <v>5</v>
+        <v>10.63</v>
       </c>
       <c r="F7" s="7">
         <f>SUM(G7:M7)</f>
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="G7" s="1">
         <v>1</v>
@@ -1863,7 +1852,9 @@
       <c r="H7" s="1">
         <v>6</v>
       </c>
-      <c r="I7" s="1"/>
+      <c r="I7" s="1">
+        <v>10</v>
+      </c>
       <c r="J7" s="1"/>
     </row>
     <row r="8" spans="2:10" ht="15.75" x14ac:dyDescent="0.2">
@@ -1871,22 +1862,28 @@
         <v>2</v>
       </c>
       <c r="C8" s="7">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D8" s="1">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="E8" s="1">
         <f t="shared" ref="E8:E11" si="0">(F8/D8)*C8</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="F8" s="7">
         <f t="shared" ref="F8:F11" si="1">SUM(G8:M8)</f>
-        <v>0</v>
-      </c>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
+        <v>28</v>
+      </c>
+      <c r="G8" s="1">
+        <v>8</v>
+      </c>
+      <c r="H8" s="1">
+        <v>10</v>
+      </c>
+      <c r="I8" s="1">
+        <v>10</v>
+      </c>
       <c r="J8" s="1"/>
     </row>
     <row r="9" spans="2:10" ht="15.75" x14ac:dyDescent="0.2">
@@ -1939,24 +1936,24 @@
     </row>
     <row r="11" spans="2:10" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B11" s="7" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C11" s="7">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D11" s="1">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E11" s="1">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="F11" s="7">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="G11" s="1">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
@@ -1977,7 +1974,7 @@
       <c r="D13" s="7"/>
       <c r="E13" s="7">
         <f>ROUND(SUM(E6:E11),2)</f>
-        <v>38.56</v>
+        <v>47.19</v>
       </c>
       <c r="F13" s="1" t="str">
         <f>IF(E13&gt;86,"A",IF(E13&gt;82,"A-",IF(E13&gt;78,"B+",IF(E13&gt;74,"B",IF(E13&gt;70,"B-",IF(E13&gt;66,"C+",IF(E13&gt;62,"C",IF(E13&gt;58,"C-","F"))))))))</f>

</xml_diff>

<commit_message>
working on TDD project
</commit_message>
<xml_diff>
--- a/Marks.xlsx
+++ b/Marks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DarkJoker\Desktop\Semeste_6_FALL-2021_\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C2EBC40-53FD-41AE-B2F6-B7B3903B9F1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E896BF00-7FCD-46C9-B425-A494029F4A1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GPA" sheetId="7" r:id="rId1"/>
@@ -1123,8 +1123,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B5:J15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1200,18 +1200,22 @@
         <v>10</v>
       </c>
       <c r="D8" s="1">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="E8" s="1">
         <f>ROUND((F8/D8)*C8,2)</f>
-        <v>0</v>
+        <v>8.5</v>
       </c>
       <c r="F8" s="2">
         <f>SUM(G8:M8)</f>
-        <v>0</v>
-      </c>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
+        <v>17</v>
+      </c>
+      <c r="G8" s="1">
+        <v>8</v>
+      </c>
+      <c r="H8" s="1">
+        <v>9</v>
+      </c>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
     </row>
@@ -1223,18 +1227,22 @@
         <v>10</v>
       </c>
       <c r="D9" s="1">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="E9" s="1">
         <f t="shared" ref="E9:E12" si="0">(F9/D9)*C9</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F9" s="2">
         <f t="shared" ref="F9:F12" si="1">SUM(G9:M9)</f>
-        <v>0</v>
-      </c>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
+        <v>20</v>
+      </c>
+      <c r="G9" s="1">
+        <v>10</v>
+      </c>
+      <c r="H9" s="1">
+        <v>10</v>
+      </c>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
     </row>
@@ -1333,7 +1341,7 @@
       <c r="D14" s="2"/>
       <c r="E14" s="2">
         <f>ROUND(SUM(E7:E12),2)</f>
-        <v>18.8</v>
+        <v>37.299999999999997</v>
       </c>
       <c r="F14" s="1" t="str">
         <f>IF(E14&gt;86,"A",IF(E14&gt;82,"A-",IF(E14&gt;78,"B+",IF(E14&gt;74,"B",IF(E14&gt;70,"B-",IF(E14&gt;66,"C+",IF(E14&gt;62,"C",IF(E14&gt;58,"C-","F"))))))))</f>
@@ -1576,7 +1584,7 @@
   <dimension ref="B5:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11:G11"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1619,17 +1627,19 @@
         <v>10</v>
       </c>
       <c r="D6" s="1">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="E6" s="1">
         <f>(F6/D6)*C6</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F6" s="7">
         <f>SUM(G6:M6)</f>
-        <v>0</v>
-      </c>
-      <c r="G6" s="1"/>
+        <v>16</v>
+      </c>
+      <c r="G6" s="1">
+        <v>16</v>
+      </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
@@ -1671,21 +1681,25 @@
         <v>15</v>
       </c>
       <c r="D8" s="1">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E8" s="1">
-        <f t="shared" ref="E8:E11" si="0">(F8/D8)*C8</f>
-        <v>15</v>
+        <f t="shared" ref="E8:E10" si="0">(F8/D8)*C8</f>
+        <v>14.5</v>
       </c>
       <c r="F8" s="2">
-        <f t="shared" ref="F8:F11" si="1">SUM(G8:M8)</f>
-        <v>20</v>
+        <f t="shared" ref="F8:F10" si="1">SUM(G8:M8)</f>
+        <v>58</v>
       </c>
       <c r="G8" s="1">
         <v>20</v>
       </c>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
+      <c r="H8" s="1">
+        <v>18</v>
+      </c>
+      <c r="I8" s="1">
+        <v>20</v>
+      </c>
       <c r="J8" s="1"/>
     </row>
     <row r="9" spans="2:10" ht="15.75" x14ac:dyDescent="0.2">
@@ -1762,7 +1776,7 @@
       <c r="D13" s="2"/>
       <c r="E13" s="2">
         <f>ROUND(SUM(E6:E11),2)</f>
-        <v>42.5</v>
+        <v>50</v>
       </c>
       <c r="F13" s="1" t="str">
         <f>IF(E13&gt;86,"A",IF(E13&gt;82,"A-",IF(E13&gt;78,"B+",IF(E13&gt;74,"B",IF(E13&gt;70,"B-",IF(E13&gt;66,"C+",IF(E13&gt;62,"C",IF(E13&gt;58,"C-","F"))))))))</f>
@@ -1782,8 +1796,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAAB841F-FB29-4B50-A6D0-F2C50CE00124}">
   <dimension ref="B5:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:G6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
MFY auto commit at 17/06/2022 23:25:12
</commit_message>
<xml_diff>
--- a/Marks.xlsx
+++ b/Marks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DarkJoker\Desktop\Semeste_6_FALL-2021_\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D92546F-6651-4729-B65A-2027F26F469E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E649B240-5F24-412E-8D5C-D0A22BFDEEDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GPA" sheetId="7" r:id="rId1"/>
@@ -186,7 +186,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -219,6 +219,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -503,8 +506,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C4:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -560,7 +563,7 @@
       </c>
       <c r="G7" s="5" t="str">
         <f>IOT!F12</f>
-        <v>C+</v>
+        <v>A</v>
       </c>
       <c r="H7" s="5" t="str">
         <f>SQE!F13</f>
@@ -589,7 +592,7 @@
       </c>
       <c r="G8" s="5">
         <f>IF(G7 = "A", 4, IF(G7 = "A-", 3.67, IF(G7 = "B+", 3.33, IF(G7 = "B", 3, IF(G7 = "B-", 2.67, IF(G7 = "C+", 2.33, IF(G7 = "C",2,  IF(G7 = "C-", 1.67, 0))))))))</f>
-        <v>2.33</v>
+        <v>4</v>
       </c>
       <c r="H8" s="5">
         <f>IF(H7 = "A", 4, IF(H7 = "A-", 3.67, IF(H7 = "B+", 3.33, IF(H7 = "B", 3, IF(H7 = "B-", 2.67, IF(H7 = "C+", 2.33, IF(H7 = "C",2,  IF(H7 = "C-", 1.67, 0))))))))</f>
@@ -601,7 +604,7 @@
       </c>
       <c r="J8" s="5">
         <f>SUM(D8:I8)</f>
-        <v>6</v>
+        <v>7.67</v>
       </c>
     </row>
     <row r="9" spans="3:10" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -609,26 +612,32 @@
         <v>17</v>
       </c>
       <c r="D9" s="5">
+        <f t="shared" ref="D9:E9" si="1">IF(D8=0, 0,3)</f>
+        <v>0</v>
+      </c>
+      <c r="E9" s="5">
+        <f t="shared" ref="E9" si="2">IF(E8=0, 0,3)</f>
+        <v>0</v>
+      </c>
+      <c r="F9" s="5">
+        <f t="shared" ref="F9" si="3">IF(F8=0, 0,3)</f>
+        <v>0</v>
+      </c>
+      <c r="G9" s="5">
+        <f t="shared" ref="G9" si="4">IF(G8=0, 0,3)</f>
         <v>3</v>
       </c>
-      <c r="E9" s="5">
+      <c r="H9" s="5">
+        <f t="shared" ref="H9" si="5">IF(H8=0, 0,3)</f>
         <v>3</v>
       </c>
-      <c r="F9" s="5">
-        <v>3</v>
-      </c>
-      <c r="G9" s="5">
-        <v>3</v>
-      </c>
-      <c r="H9" s="5">
-        <v>3</v>
-      </c>
       <c r="I9" s="5">
-        <v>3</v>
+        <f t="shared" ref="I9" si="6">IF(I8=0, 0,3)</f>
+        <v>0</v>
       </c>
       <c r="J9" s="5">
         <f>SUM(D9:I9)</f>
-        <v>18</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="3:10" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -640,7 +649,7 @@
         <v>0</v>
       </c>
       <c r="E10" s="5">
-        <f t="shared" ref="E10:I10" si="1">E8*E9</f>
+        <f t="shared" ref="E10:I10" si="7">E8*E9</f>
         <v>0</v>
       </c>
       <c r="F10" s="5">
@@ -649,19 +658,19 @@
       </c>
       <c r="G10" s="5">
         <f>G8*G9</f>
-        <v>6.99</v>
+        <v>12</v>
       </c>
       <c r="H10" s="5">
         <f>H8*H9</f>
         <v>11.01</v>
       </c>
       <c r="I10" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="J10" s="5">
         <f>SUM(D10:I10)</f>
-        <v>18</v>
+        <v>23.009999999999998</v>
       </c>
     </row>
     <row r="12" spans="3:10" x14ac:dyDescent="0.2">
@@ -670,7 +679,7 @@
       </c>
       <c r="I12" s="5">
         <f>(J10/J9)</f>
-        <v>1</v>
+        <v>3.8349999999999995</v>
       </c>
     </row>
     <row r="13" spans="3:10" x14ac:dyDescent="0.2">
@@ -687,7 +696,7 @@
   <dimension ref="B4:J16"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16:E17"/>
+      <selection activeCell="G8" sqref="G8:G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.2"/>
@@ -700,12 +709,12 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="G4" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
+      <c r="G4" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12"/>
     </row>
     <row r="5" spans="2:10" ht="31.5" x14ac:dyDescent="0.2">
       <c r="C5" s="2" t="s">
@@ -861,7 +870,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B5:N15"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B4" workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
@@ -1024,7 +1033,7 @@
         <v>0</v>
       </c>
       <c r="F10" s="2">
-        <f t="shared" ref="F9:F11" si="1">SUM(G10:M10)</f>
+        <f t="shared" ref="F10:F11" si="1">SUM(G10:M10)</f>
         <v>0</v>
       </c>
       <c r="G10" s="1"/>
@@ -1120,7 +1129,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B5:J15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
@@ -1251,17 +1260,19 @@
         <v>40</v>
       </c>
       <c r="D10" s="1">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="E10" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>32.400000000000006</v>
       </c>
       <c r="F10" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G10" s="1"/>
+        <v>81</v>
+      </c>
+      <c r="G10" s="1">
+        <v>81</v>
+      </c>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
@@ -1278,15 +1289,13 @@
       </c>
       <c r="E11" s="1">
         <f t="shared" si="0"/>
-        <v>18.799999999999997</v>
+        <v>0</v>
       </c>
       <c r="F11" s="2">
         <f t="shared" si="1"/>
-        <v>47</v>
-      </c>
-      <c r="G11" s="1">
-        <v>47</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
@@ -1336,7 +1345,7 @@
       <c r="D14" s="2"/>
       <c r="E14" s="2">
         <f>ROUND(SUM(E7:E12),2)</f>
-        <v>33.799999999999997</v>
+        <v>47.4</v>
       </c>
       <c r="F14" s="1" t="str">
         <f>IF(E14&gt;86,"A",IF(E14&gt;82,"A-",IF(E14&gt;78,"B+",IF(E14&gt;74,"B",IF(E14&gt;70,"B-",IF(E14&gt;66,"C+",IF(E14&gt;62,"C",IF(E14&gt;58,"C-","F"))))))))</f>
@@ -1367,7 +1376,7 @@
   <dimension ref="B5:J60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1407,20 +1416,22 @@
         <v>0</v>
       </c>
       <c r="C6" s="7">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D6" s="1">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="E6" s="1">
         <f>(F6/D6)*C6</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="F6" s="7">
         <f>SUM(G6:M6)</f>
-        <v>0</v>
-      </c>
-      <c r="G6" s="1"/>
+        <v>20</v>
+      </c>
+      <c r="G6" s="1">
+        <v>20</v>
+      </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
@@ -1469,7 +1480,7 @@
         <v>10</v>
       </c>
       <c r="F8" s="2">
-        <f t="shared" ref="F8:F10" si="1">SUM(G8:M8)</f>
+        <f t="shared" ref="F8:F11" si="1">SUM(G8:M8)</f>
         <v>20</v>
       </c>
       <c r="G8" s="1">
@@ -1533,7 +1544,7 @@
     </row>
     <row r="11" spans="2:10" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
+      <c r="C11" s="10"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="2"/>
@@ -1547,17 +1558,17 @@
         <v>11</v>
       </c>
       <c r="C12" s="2">
-        <f>SUM(C7:C10)</f>
-        <v>80</v>
+        <f>SUM(C6:C11)</f>
+        <v>100</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2">
-        <f>ROUND(SUM(E6:E10),2)</f>
-        <v>68.5</v>
+        <f>ROUND(SUM(E6:E11),2)</f>
+        <v>88.5</v>
       </c>
       <c r="F12" s="1" t="str">
         <f>IF(E12&gt;86,"A",IF(E12&gt;82,"A-",IF(E12&gt;78,"B+",IF(E12&gt;74,"B",IF(E12&gt;70,"B-",IF(E12&gt;66,"C+",IF(E12&gt;62,"C",IF(E12&gt;58,"C-","F"))))))))</f>
-        <v>C+</v>
+        <v>A</v>
       </c>
       <c r="G12" s="2"/>
       <c r="H12" s="1"/>
@@ -1803,7 +1814,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAAB841F-FB29-4B50-A6D0-F2C50CE00124}">
   <dimension ref="B5:J13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
MFY auto commit at 20/06/2022 23:54:27
</commit_message>
<xml_diff>
--- a/Marks.xlsx
+++ b/Marks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DarkJoker\Desktop\Semeste_6_FALL-2021_\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E649B240-5F24-412E-8D5C-D0A22BFDEEDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E05E08B-C665-408B-9838-1D729EB03777}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GPA" sheetId="7" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="32">
   <si>
     <t>Project</t>
   </si>
@@ -114,6 +114,24 @@
   </si>
   <si>
     <t>Final</t>
+  </si>
+  <si>
+    <t>Extra</t>
+  </si>
+  <si>
+    <t>Last Semester</t>
+  </si>
+  <si>
+    <t>Last Semester Creadit hours</t>
+  </si>
+  <si>
+    <t>Semester CGPA</t>
+  </si>
+  <si>
+    <t>Total CGPA</t>
+  </si>
+  <si>
+    <t>Total CR</t>
   </si>
 </sst>
 </file>
@@ -186,7 +204,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -196,15 +214,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -222,6 +231,18 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -504,186 +525,246 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C4:J13"/>
+  <dimension ref="C4:M22"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" style="5"/>
-    <col min="2" max="2" width="10.28515625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" style="5" customWidth="1"/>
-    <col min="4" max="16384" width="12.7109375" style="5"/>
+    <col min="1" max="1" width="12.7109375" style="12"/>
+    <col min="2" max="2" width="10.28515625" style="12" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" style="12" customWidth="1"/>
+    <col min="4" max="10" width="12.7109375" style="12"/>
+    <col min="11" max="11" width="12.7109375" style="11"/>
+    <col min="12" max="12" width="12.7109375" style="12"/>
+    <col min="13" max="13" width="16.42578125" style="11" customWidth="1"/>
+    <col min="14" max="16384" width="12.7109375" style="12"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C4" s="4"/>
-      <c r="D4" s="4" t="s">
+    <row r="4" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C4" s="10"/>
+      <c r="D4" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="H4" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="I4" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="J4" s="4" t="s">
+      <c r="J4" s="10" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C5" s="4"/>
-    </row>
-    <row r="7" spans="3:10" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C7" s="4" t="s">
+    <row r="5" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C5" s="10"/>
+    </row>
+    <row r="7" spans="3:13" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C7" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="5" t="str">
+      <c r="D7" s="12" t="str">
         <f>WE!F14</f>
         <v>F</v>
       </c>
-      <c r="E7" s="5" t="str">
+      <c r="E7" s="12" t="str">
         <f>OR!F14</f>
-        <v>F</v>
-      </c>
-      <c r="F7" s="5" t="str">
+        <v>A</v>
+      </c>
+      <c r="F7" s="12" t="str">
         <f>TDD!F14</f>
         <v>F</v>
       </c>
-      <c r="G7" s="5" t="str">
+      <c r="G7" s="12" t="str">
         <f>IOT!F12</f>
         <v>A</v>
       </c>
-      <c r="H7" s="5" t="str">
+      <c r="H7" s="12" t="str">
         <f>SQE!F13</f>
-        <v>A-</v>
-      </c>
-      <c r="I7" s="6" t="str">
+        <v>A</v>
+      </c>
+      <c r="I7" s="13" t="str">
         <f>HCI!F13</f>
         <v>F</v>
       </c>
     </row>
-    <row r="8" spans="3:10" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C8" s="4" t="s">
+    <row r="8" spans="3:13" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C8" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="12">
         <f>IF(D7 = "A", 4, IF(D7 = "A-", 3.67, IF(D7 = "B+", 3.33, IF(D7 = "B", 3, IF(D7 = "B-", 2.67, IF(D7 = "C+", 2.33, IF(D7 = "C",2,  IF(D7 = "C-", 1.67, 0))))))))</f>
         <v>0</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="12">
         <f t="shared" ref="E8:I8" si="0">IF(E7 = "A", 4, IF(E7 = "A-", 3.67, IF(E7 = "B+", 3.33, IF(E7 = "B", 3, IF(E7 = "B-", 2.67, IF(E7 = "C+", 2.33, IF(E7 = "C",2,  IF(E7 = "C-", 1.67, 0))))))))</f>
-        <v>0</v>
-      </c>
-      <c r="F8" s="5">
+        <v>4</v>
+      </c>
+      <c r="F8" s="12">
         <f>IF(F7 = "A", 4, IF(F7 = "A-", 3.67, IF(F7 = "B+", 3.33, IF(F7 = "B", 3, IF(F7 = "B-", 2.67, IF(F7 = "C+", 2.33, IF(F7 = "C",2,  IF(F7 = "C-", 1.67, 0))))))))</f>
         <v>0</v>
       </c>
-      <c r="G8" s="5">
+      <c r="G8" s="12">
         <f>IF(G7 = "A", 4, IF(G7 = "A-", 3.67, IF(G7 = "B+", 3.33, IF(G7 = "B", 3, IF(G7 = "B-", 2.67, IF(G7 = "C+", 2.33, IF(G7 = "C",2,  IF(G7 = "C-", 1.67, 0))))))))</f>
         <v>4</v>
       </c>
-      <c r="H8" s="5">
+      <c r="H8" s="12">
         <f>IF(H7 = "A", 4, IF(H7 = "A-", 3.67, IF(H7 = "B+", 3.33, IF(H7 = "B", 3, IF(H7 = "B-", 2.67, IF(H7 = "C+", 2.33, IF(H7 = "C",2,  IF(H7 = "C-", 1.67, 0))))))))</f>
-        <v>3.67</v>
-      </c>
-      <c r="I8" s="5">
+        <v>4</v>
+      </c>
+      <c r="I8" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J8" s="5">
+      <c r="J8" s="12">
         <f>SUM(D8:I8)</f>
-        <v>7.67</v>
-      </c>
-    </row>
-    <row r="9" spans="3:10" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="M8" s="12"/>
+    </row>
+    <row r="9" spans="3:13" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C9" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="5">
-        <f t="shared" ref="D9:E9" si="1">IF(D8=0, 0,3)</f>
-        <v>0</v>
-      </c>
-      <c r="E9" s="5">
+      <c r="D9" s="12">
+        <f t="shared" ref="D9" si="1">IF(D8=0, 0,3)</f>
+        <v>0</v>
+      </c>
+      <c r="E9" s="12">
         <f t="shared" ref="E9" si="2">IF(E8=0, 0,3)</f>
-        <v>0</v>
-      </c>
-      <c r="F9" s="5">
+        <v>3</v>
+      </c>
+      <c r="F9" s="12">
         <f t="shared" ref="F9" si="3">IF(F8=0, 0,3)</f>
         <v>0</v>
       </c>
-      <c r="G9" s="5">
+      <c r="G9" s="12">
         <f t="shared" ref="G9" si="4">IF(G8=0, 0,3)</f>
         <v>3</v>
       </c>
-      <c r="H9" s="5">
+      <c r="H9" s="12">
         <f t="shared" ref="H9" si="5">IF(H8=0, 0,3)</f>
         <v>3</v>
       </c>
-      <c r="I9" s="5">
+      <c r="I9" s="12">
         <f t="shared" ref="I9" si="6">IF(I8=0, 0,3)</f>
         <v>0</v>
       </c>
-      <c r="J9" s="5">
+      <c r="J9" s="12">
         <f>SUM(D9:I9)</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="3:10" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C10" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="M9" s="12"/>
+    </row>
+    <row r="10" spans="3:13" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C10" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="12">
         <f>D8*D9</f>
         <v>0</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="12">
         <f t="shared" ref="E10:I10" si="7">E8*E9</f>
-        <v>0</v>
-      </c>
-      <c r="F10" s="5">
+        <v>12</v>
+      </c>
+      <c r="F10" s="12">
         <f>F8*F9</f>
         <v>0</v>
       </c>
-      <c r="G10" s="5">
+      <c r="G10" s="12">
         <f>G8*G9</f>
         <v>12</v>
       </c>
-      <c r="H10" s="5">
+      <c r="H10" s="12">
         <f>H8*H9</f>
-        <v>11.01</v>
-      </c>
-      <c r="I10" s="5">
+        <v>12</v>
+      </c>
+      <c r="I10" s="12">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="J10" s="5">
+      <c r="J10" s="12">
         <f>SUM(D10:I10)</f>
-        <v>23.009999999999998</v>
-      </c>
-    </row>
-    <row r="12" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="H12" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="M10" s="12"/>
+    </row>
+    <row r="12" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="H12" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="I12" s="5">
+      <c r="I12" s="12">
         <f>(J10/J9)</f>
-        <v>3.8349999999999995</v>
-      </c>
-    </row>
-    <row r="13" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C13" s="6"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C13" s="13"/>
+    </row>
+    <row r="15" spans="3:13" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="C15" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" s="12">
+        <f>I12*D16</f>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C16" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" s="12">
+        <f>J9</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C18" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D18" s="12">
+        <f>ROUND(3.62*D19,2)</f>
+        <v>311.32</v>
+      </c>
+    </row>
+    <row r="19" spans="3:4" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="C19" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D19" s="12">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="21" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C21" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D21" s="12">
+        <f>ROUND((D15+D18)/D22, 2)</f>
+        <v>3.66</v>
+      </c>
+    </row>
+    <row r="22" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C22" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D22" s="12">
+        <f>D16+D19</f>
+        <v>95</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -696,7 +777,7 @@
   <dimension ref="B4:J16"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8:G10"/>
+      <selection activeCell="G10" sqref="G8:G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.2"/>
@@ -709,12 +790,12 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="G4" s="12" t="s">
+      <c r="G4" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
     </row>
     <row r="5" spans="2:10" ht="31.5" x14ac:dyDescent="0.2">
       <c r="C5" s="2" t="s">
@@ -760,7 +841,7 @@
         <f>SUM(G7:J7)</f>
         <v>17</v>
       </c>
-      <c r="G7" s="11">
+      <c r="G7" s="8">
         <v>17</v>
       </c>
     </row>
@@ -778,7 +859,7 @@
         <f t="shared" ref="E8:E10" si="0">(F8/D8)*C8</f>
         <v>0</v>
       </c>
-      <c r="F8" s="9">
+      <c r="F8" s="6">
         <f t="shared" ref="F8:F10" si="1">SUM(G8:J8)</f>
         <v>0</v>
       </c>
@@ -797,7 +878,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F9" s="9">
+      <c r="F9" s="6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -816,15 +897,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F10" s="9">
-        <f t="shared" si="1"/>
+      <c r="F10" s="6">
+        <f>SUM(G10:J10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B11" s="2"/>
       <c r="E11" s="1"/>
-      <c r="F11" s="8"/>
+      <c r="F11" s="5"/>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B12" s="2"/>
@@ -871,7 +952,7 @@
   <dimension ref="B5:N15"/>
   <sheetViews>
     <sheetView topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -905,16 +986,16 @@
       <c r="J5" s="1">
         <v>4</v>
       </c>
-      <c r="K5" s="8">
+      <c r="K5" s="5">
         <v>5</v>
       </c>
-      <c r="L5" s="8">
+      <c r="L5" s="5">
         <v>6</v>
       </c>
-      <c r="M5" s="8">
+      <c r="M5" s="5">
         <v>7</v>
       </c>
-      <c r="N5" s="8">
+      <c r="N5" s="5">
         <v>8</v>
       </c>
     </row>
@@ -947,15 +1028,15 @@
         <v>15</v>
       </c>
       <c r="D8" s="1">
-        <v>95</v>
+        <v>115</v>
       </c>
       <c r="E8" s="1">
         <f>ROUND((F8/D8)*C8,2)</f>
-        <v>14.37</v>
+        <v>14.22</v>
       </c>
       <c r="F8" s="2">
         <f>SUM(G8:M8)</f>
-        <v>91</v>
+        <v>109</v>
       </c>
       <c r="G8" s="1">
         <v>10</v>
@@ -967,12 +1048,14 @@
         <v>14</v>
       </c>
       <c r="J8" s="1">
+        <v>18</v>
+      </c>
+      <c r="K8" s="1">
         <v>30</v>
       </c>
-      <c r="K8" s="1">
+      <c r="L8" s="1">
         <v>20</v>
       </c>
-      <c r="L8" s="1"/>
       <c r="M8" s="1"/>
     </row>
     <row r="9" spans="2:14" ht="15.75" x14ac:dyDescent="0.2">
@@ -986,8 +1069,8 @@
         <v>360</v>
       </c>
       <c r="E9" s="1">
-        <f t="shared" ref="E9:E11" si="0">(F9/D9)*C9</f>
-        <v>13.208333333333332</v>
+        <f>ROUND((F9/D9)*C9, 2)</f>
+        <v>13.21</v>
       </c>
       <c r="F9" s="2">
         <f>SUM(G9:N9)</f>
@@ -1029,14 +1112,16 @@
         <v>100</v>
       </c>
       <c r="E10" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" ref="E10:E11" si="0">(F10/D10)*C10</f>
+        <v>46</v>
       </c>
       <c r="F10" s="2">
         <f t="shared" ref="F10:F11" si="1">SUM(G10:M10)</f>
-        <v>0</v>
-      </c>
-      <c r="G10" s="1"/>
+        <v>92</v>
+      </c>
+      <c r="G10" s="1">
+        <v>92</v>
+      </c>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
@@ -1099,11 +1184,11 @@
       <c r="D14" s="2"/>
       <c r="E14" s="2">
         <f>ROUND(SUM(E7:E12),2)</f>
-        <v>46.08</v>
+        <v>91.93</v>
       </c>
       <c r="F14" s="1" t="str">
         <f>IF(E14&gt;86,"A",IF(E14&gt;82,"A-",IF(E14&gt;78,"B+",IF(E14&gt;74,"B",IF(E14&gt;70,"B-",IF(E14&gt;66,"C+",IF(E14&gt;62,"C",IF(E14&gt;58,"C-","F"))))))))</f>
-        <v>F</v>
+        <v>A</v>
       </c>
       <c r="G14" s="2"/>
       <c r="H14" s="1"/>
@@ -1129,7 +1214,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B5:J15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
@@ -1264,15 +1349,13 @@
       </c>
       <c r="E10" s="1">
         <f t="shared" si="0"/>
-        <v>32.400000000000006</v>
+        <v>0</v>
       </c>
       <c r="F10" s="2">
         <f t="shared" si="1"/>
-        <v>81</v>
-      </c>
-      <c r="G10" s="1">
-        <v>81</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
@@ -1289,13 +1372,15 @@
       </c>
       <c r="E11" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>18.799999999999997</v>
       </c>
       <c r="F11" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G11" s="1"/>
+        <v>47</v>
+      </c>
+      <c r="G11" s="1">
+        <v>47</v>
+      </c>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
@@ -1345,7 +1430,7 @@
       <c r="D14" s="2"/>
       <c r="E14" s="2">
         <f>ROUND(SUM(E7:E12),2)</f>
-        <v>47.4</v>
+        <v>33.799999999999997</v>
       </c>
       <c r="F14" s="1" t="str">
         <f>IF(E14&gt;86,"A",IF(E14&gt;82,"A-",IF(E14&gt;78,"B+",IF(E14&gt;74,"B",IF(E14&gt;70,"B-",IF(E14&gt;66,"C+",IF(E14&gt;62,"C",IF(E14&gt;58,"C-","F"))))))))</f>
@@ -1412,10 +1497,10 @@
       </c>
     </row>
     <row r="6" spans="2:10" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="B6" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C6" s="7">
+      <c r="B6" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="4">
         <v>20</v>
       </c>
       <c r="D6" s="1">
@@ -1425,7 +1510,7 @@
         <f>(F6/D6)*C6</f>
         <v>20</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F6" s="4">
         <f>SUM(G6:M6)</f>
         <v>20</v>
       </c>
@@ -1480,7 +1565,7 @@
         <v>10</v>
       </c>
       <c r="F8" s="2">
-        <f t="shared" ref="F8:F11" si="1">SUM(G8:M8)</f>
+        <f t="shared" ref="F8:F10" si="1">SUM(G8:M8)</f>
         <v>20</v>
       </c>
       <c r="G8" s="1">
@@ -1544,7 +1629,7 @@
     </row>
     <row r="11" spans="2:10" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B11" s="1"/>
-      <c r="C11" s="10"/>
+      <c r="C11" s="7"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="2"/>
@@ -1600,7 +1685,7 @@
   <dimension ref="B5:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1636,10 +1721,10 @@
       </c>
     </row>
     <row r="6" spans="2:10" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="B6" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C6" s="7">
+      <c r="B6" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="4">
         <v>10</v>
       </c>
       <c r="D6" s="1">
@@ -1649,7 +1734,7 @@
         <f>(F6/D6)*C6</f>
         <v>8</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F6" s="4">
         <f>SUM(G6:M6)</f>
         <v>16</v>
       </c>
@@ -1769,11 +1854,15 @@
       <c r="J10" s="1"/>
     </row>
     <row r="11" spans="2:10" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
+      <c r="B11" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="4"/>
       <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="7"/>
+      <c r="E11" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="F11" s="4"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
@@ -1794,11 +1883,11 @@
       <c r="D13" s="2"/>
       <c r="E13" s="2">
         <f>ROUND(SUM(E6:E11),2)</f>
-        <v>84</v>
+        <v>86.5</v>
       </c>
       <c r="F13" s="1" t="str">
         <f>IF(E13&gt;86,"A",IF(E13&gt;82,"A-",IF(E13&gt;78,"B+",IF(E13&gt;74,"B",IF(E13&gt;70,"B-",IF(E13&gt;66,"C+",IF(E13&gt;62,"C",IF(E13&gt;58,"C-","F"))))))))</f>
-        <v>A-</v>
+        <v>A</v>
       </c>
       <c r="G13" s="2"/>
       <c r="H13" s="1"/>
@@ -1825,25 +1914,25 @@
   <sheetData>
     <row r="5" spans="2:10" ht="31.5" x14ac:dyDescent="0.2">
       <c r="B5" s="1"/>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="7">
+      <c r="G5" s="4">
         <v>1</v>
       </c>
-      <c r="H5" s="7">
+      <c r="H5" s="4">
         <v>2</v>
       </c>
-      <c r="I5" s="7">
+      <c r="I5" s="4">
         <v>3</v>
       </c>
       <c r="J5" s="1">
@@ -1851,20 +1940,20 @@
       </c>
     </row>
     <row r="6" spans="2:10" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="C6" s="7"/>
+      <c r="C6" s="4"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
-      <c r="F6" s="7"/>
+      <c r="F6" s="4"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
     </row>
     <row r="7" spans="2:10" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="4">
         <v>15</v>
       </c>
       <c r="D7" s="1">
@@ -1874,7 +1963,7 @@
         <f>ROUND((F7/D7)*C7,2)</f>
         <v>10.63</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="4">
         <f>SUM(G7:M7)</f>
         <v>17</v>
       </c>
@@ -1890,10 +1979,10 @@
       <c r="J7" s="1"/>
     </row>
     <row r="8" spans="2:10" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C8" s="4">
         <v>15</v>
       </c>
       <c r="D8" s="1">
@@ -1903,7 +1992,7 @@
         <f t="shared" ref="E8:E11" si="0">(F8/D8)*C8</f>
         <v>14</v>
       </c>
-      <c r="F8" s="7">
+      <c r="F8" s="4">
         <f t="shared" ref="F8:F11" si="1">SUM(G8:M8)</f>
         <v>28</v>
       </c>
@@ -1919,10 +2008,10 @@
       <c r="J8" s="1"/>
     </row>
     <row r="9" spans="2:10" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="4">
         <v>40</v>
       </c>
       <c r="D9" s="1">
@@ -1932,7 +2021,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F9" s="7">
+      <c r="F9" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1942,10 +2031,10 @@
       <c r="J9" s="1"/>
     </row>
     <row r="10" spans="2:10" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C10" s="4">
         <v>20</v>
       </c>
       <c r="D10" s="1">
@@ -1955,7 +2044,7 @@
         <f t="shared" si="0"/>
         <v>13.555555555555557</v>
       </c>
-      <c r="F10" s="7">
+      <c r="F10" s="4">
         <f t="shared" si="1"/>
         <v>61</v>
       </c>
@@ -1967,10 +2056,10 @@
       <c r="J10" s="1"/>
     </row>
     <row r="11" spans="2:10" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="B11" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C11" s="7">
+      <c r="B11" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="4">
         <v>10</v>
       </c>
       <c r="D11" s="1">
@@ -1980,7 +2069,7 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="F11" s="7">
+      <c r="F11" s="4">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
@@ -1996,15 +2085,15 @@
       <c r="J12" s="1"/>
     </row>
     <row r="13" spans="2:10" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="7">
+      <c r="C13" s="4">
         <f>SUM(C6:C11)</f>
         <v>100</v>
       </c>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7">
+      <c r="D13" s="4"/>
+      <c r="E13" s="4">
         <f>ROUND(SUM(E6:E11),2)</f>
         <v>47.19</v>
       </c>
@@ -2012,7 +2101,7 @@
         <f>IF(E13&gt;86,"A",IF(E13&gt;82,"A-",IF(E13&gt;78,"B+",IF(E13&gt;74,"B",IF(E13&gt;70,"B-",IF(E13&gt;66,"C+",IF(E13&gt;62,"C",IF(E13&gt;58,"C-","F"))))))))</f>
         <v>F</v>
       </c>
-      <c r="G13" s="7"/>
+      <c r="G13" s="4"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>

</xml_diff>

<commit_message>
MFY auto commit at 01/07/2022 10:15:55
</commit_message>
<xml_diff>
--- a/Marks.xlsx
+++ b/Marks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DarkJoker\Desktop\Semeste_6_FALL-2021_\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56124B01-4500-4AF3-971A-4F17C7EA2325}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D524493C-A259-4C32-9488-FEEDA3102692}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GPA" sheetId="7" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="31">
   <si>
     <t>Project</t>
   </si>
@@ -201,7 +201,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -237,6 +237,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -524,8 +530,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C4:M22"/>
   <sheetViews>
-    <sheetView topLeftCell="C4" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -593,7 +599,7 @@
       </c>
       <c r="I7" s="12" t="str">
         <f>HCI!F13</f>
-        <v>F</v>
+        <v>A</v>
       </c>
     </row>
     <row r="8" spans="3:13" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -622,11 +628,11 @@
       </c>
       <c r="I8" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J8" s="11">
         <f>SUM(D8:I8)</f>
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="M8" s="11"/>
     </row>
@@ -656,11 +662,11 @@
       </c>
       <c r="I9" s="11">
         <f t="shared" ref="I9" si="6">IF(I8=0, 0,3)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J9" s="11">
         <f>SUM(D9:I9)</f>
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="M9" s="11"/>
     </row>
@@ -690,11 +696,11 @@
       </c>
       <c r="I10" s="11">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="J10" s="11">
         <f>SUM(D10:I10)</f>
-        <v>60</v>
+        <v>72</v>
       </c>
       <c r="M10" s="11"/>
     </row>
@@ -716,7 +722,7 @@
       </c>
       <c r="D15" s="11">
         <f>I12*D16</f>
-        <v>60</v>
+        <v>72</v>
       </c>
     </row>
     <row r="16" spans="3:13" x14ac:dyDescent="0.2">
@@ -725,7 +731,7 @@
       </c>
       <c r="D16" s="11">
         <f>J9</f>
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="3:4" x14ac:dyDescent="0.2">
@@ -734,7 +740,7 @@
       </c>
       <c r="D18" s="11">
         <f>ROUND(3.62*D19,2)</f>
-        <v>311.32</v>
+        <v>300.45999999999998</v>
       </c>
     </row>
     <row r="19" spans="3:4" ht="25.5" x14ac:dyDescent="0.2">
@@ -742,7 +748,7 @@
         <v>27</v>
       </c>
       <c r="D19" s="11">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="21" spans="3:4" x14ac:dyDescent="0.2">
@@ -751,7 +757,7 @@
       </c>
       <c r="D21" s="11">
         <f>ROUND((D15+D18)/D22, 2)</f>
-        <v>3.68</v>
+        <v>3.69</v>
       </c>
     </row>
     <row r="22" spans="3:4" x14ac:dyDescent="0.2">
@@ -774,7 +780,7 @@
   <dimension ref="B4:J16"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.2"/>
@@ -787,12 +793,12 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="G4" s="13" t="s">
+      <c r="G4" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
     </row>
     <row r="5" spans="2:10" ht="31.5" x14ac:dyDescent="0.2">
       <c r="C5" s="2" t="s">
@@ -859,15 +865,15 @@
         <v>30</v>
       </c>
       <c r="E9" s="1">
-        <f t="shared" ref="E8:E10" si="0">(F9/D9)*C9</f>
-        <v>24.1</v>
+        <f t="shared" ref="E9:E10" si="0">(F9/D9)*C9</f>
+        <v>30</v>
       </c>
       <c r="F9" s="6">
-        <f t="shared" ref="F8:F9" si="1">SUM(G9:J9)</f>
-        <v>24.1</v>
+        <f t="shared" ref="F9" si="1">SUM(G9:J9)</f>
+        <v>30</v>
       </c>
       <c r="G9" s="1">
-        <v>24.1</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.2">
@@ -917,7 +923,7 @@
       <c r="D14" s="2"/>
       <c r="E14" s="3">
         <f>ROUND(SUM(E7:E12),2)</f>
-        <v>86.1</v>
+        <v>92</v>
       </c>
       <c r="F14" s="3" t="str">
         <f>IF(E14&gt;86,"A",IF(E14&gt;82,"A-",IF(E14&gt;78,"B+",IF(E14&gt;74,"B",IF(E14&gt;70,"B-",IF(E14&gt;66,"C+",IF(E14&gt;62,"C",IF(E14&gt;58,"C-","F"))))))))</f>
@@ -1204,8 +1210,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B5:J15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10:G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1341,14 +1347,14 @@
       </c>
       <c r="E10" s="1">
         <f t="shared" si="0"/>
-        <v>27.24</v>
+        <v>40</v>
       </c>
       <c r="F10" s="2">
         <f t="shared" si="1"/>
-        <v>68.099999999999994</v>
+        <v>100</v>
       </c>
       <c r="G10" s="1">
-        <v>68.099999999999994</v>
+        <v>100</v>
       </c>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
@@ -1426,7 +1432,7 @@
       <c r="D14" s="2"/>
       <c r="E14" s="2">
         <f>ROUND(SUM(E7:E12),2)</f>
-        <v>86.04</v>
+        <v>98.8</v>
       </c>
       <c r="F14" s="1" t="str">
         <f>IF(E14&gt;86,"A",IF(E14&gt;82,"A-",IF(E14&gt;78,"B+",IF(E14&gt;74,"B",IF(E14&gt;70,"B-",IF(E14&gt;66,"C+",IF(E14&gt;62,"C",IF(E14&gt;58,"C-","F"))))))))</f>
@@ -1457,7 +1463,7 @@
   <dimension ref="B5:J60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1900,12 +1906,14 @@
   <dimension ref="B5:J13"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="256" width="13.85546875" customWidth="1"/>
+    <col min="1" max="4" width="13.85546875" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" style="1" customWidth="1"/>
+    <col min="6" max="256" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="2:10" ht="31.5" x14ac:dyDescent="0.2">
@@ -1916,7 +1924,7 @@
       <c r="D5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="13" t="s">
         <v>9</v>
       </c>
       <c r="F5" s="4" t="s">
@@ -1935,29 +1943,28 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="2:10" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C6" s="4"/>
       <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
       <c r="F6" s="4"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
     </row>
-    <row r="7" spans="2:10" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B7" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C7" s="4">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D7" s="1">
         <v>24</v>
       </c>
       <c r="E7" s="1">
         <f>ROUND((F7/D7)*C7,2)</f>
-        <v>10.63</v>
+        <v>7.08</v>
       </c>
       <c r="F7" s="4">
         <f>SUM(G7:M7)</f>
@@ -1974,7 +1981,7 @@
       </c>
       <c r="J7" s="1"/>
     </row>
-    <row r="8" spans="2:10" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B8" s="4" t="s">
         <v>2</v>
       </c>
@@ -2003,7 +2010,7 @@
       </c>
       <c r="J8" s="1"/>
     </row>
-    <row r="9" spans="2:10" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B9" s="4" t="s">
         <v>3</v>
       </c>
@@ -2014,19 +2021,21 @@
         <v>180</v>
       </c>
       <c r="E9" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>ROUND(((F9/D9)*C9),2)</f>
+        <v>34.22</v>
       </c>
       <c r="F9" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G9" s="1"/>
+        <v>154</v>
+      </c>
+      <c r="G9" s="1">
+        <v>154</v>
+      </c>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
     </row>
-    <row r="10" spans="2:10" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B10" s="4" t="s">
         <v>4</v>
       </c>
@@ -2037,8 +2046,8 @@
         <v>90</v>
       </c>
       <c r="E10" s="1">
-        <f t="shared" si="0"/>
-        <v>13.555555555555557</v>
+        <f>ROUND(((F10/D10)*C10),2)</f>
+        <v>13.56</v>
       </c>
       <c r="F10" s="4">
         <f t="shared" si="1"/>
@@ -2051,51 +2060,61 @@
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
     </row>
-    <row r="11" spans="2:10" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C11" s="4">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D11" s="1">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E11" s="1">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>14.25</v>
       </c>
       <c r="F11" s="4">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="G11" s="1">
         <v>9</v>
       </c>
-      <c r="H11" s="1"/>
+      <c r="H11" s="1">
+        <v>10</v>
+      </c>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
     </row>
-    <row r="12" spans="2:10" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B12" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="13"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1">
+        <v>3</v>
+      </c>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
     </row>
-    <row r="13" spans="2:10" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B13" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C13" s="4">
-        <f>SUM(C6:C11)</f>
+        <f>SUM(C7:C12)</f>
         <v>100</v>
       </c>
       <c r="D13" s="4"/>
-      <c r="E13" s="4">
-        <f>ROUND(SUM(E6:E11),2)</f>
-        <v>47.19</v>
-      </c>
-      <c r="F13" s="1" t="str">
-        <f>IF(E13&gt;86,"A",IF(E13&gt;82,"A-",IF(E13&gt;78,"B+",IF(E13&gt;74,"B",IF(E13&gt;70,"B-",IF(E13&gt;66,"C+",IF(E13&gt;62,"C",IF(E13&gt;58,"C-","F"))))))))</f>
-        <v>F</v>
+      <c r="E13" s="14">
+        <f>ROUND(SUM(E6:E12),2)</f>
+        <v>86.11</v>
+      </c>
+      <c r="F13" s="14" t="str">
+        <f>IF(E13&gt;=86,"A",IF(E13&gt;82,"A-",IF(E13&gt;78,"B+",IF(E13&gt;74,"B",IF(E13&gt;70,"B-",IF(E13&gt;66,"C+",IF(E13&gt;62,"C",IF(E13&gt;58,"C-","F"))))))))</f>
+        <v>A</v>
       </c>
       <c r="G13" s="4"/>
       <c r="H13" s="1"/>
@@ -2104,5 +2123,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>